<commit_message>
Cleared PPP_main and updated data files
</commit_message>
<xml_diff>
--- a/Data/DiabetesPredictor-Schedule-Draft.xlsx
+++ b/Data/DiabetesPredictor-Schedule-Draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spend\Documents\Personal\ASUData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spend\Documents\Personal\ASUData\Group-Project-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FC243B-E6A6-4BB7-8E09-1E781ABF0B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C3CCE-09C2-45D8-8610-4AC9C388EBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{5F4C065F-51F9-4B62-A9A1-17C95538D7BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F4C065F-51F9-4B62-A9A1-17C95538D7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Start - Form Team / Identify tasks</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Plotting:</t>
   </si>
   <si>
-    <t>Import data</t>
-  </si>
-  <si>
     <t>Create plots per question</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
   </si>
   <si>
     <t>Work Day + Install PostgreSQL</t>
-  </si>
-  <si>
-    <t>Add cells for each activity</t>
-  </si>
-  <si>
-    <t>Add owners to each cell</t>
   </si>
   <si>
     <t>Presentation / Submission</t>
@@ -191,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +192,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -248,6 +251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="8"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +570,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,16 +585,16 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G1" s="1"/>
       <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -607,26 +612,26 @@
         <v>45324</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="G3" s="1"/>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="5">
         <v>45324</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -634,7 +639,7 @@
         <v>45327</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1"/>
       <c r="I4" s="4" t="s">
@@ -643,16 +648,22 @@
       <c r="J4" s="5">
         <v>45327</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="G5" s="1"/>
-      <c r="I5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>45329</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
@@ -661,72 +672,82 @@
         <v>45329</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="6" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="G7" s="1"/>
-      <c r="I7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="5">
-        <v>45329</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="I7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>45330</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1"/>
       <c r="I8" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>33</v>
+      <c r="K8" s="4"/>
+      <c r="L8" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="G9" s="1"/>
-      <c r="I9" s="6" t="s">
-        <v>5</v>
+      <c r="I9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>45334</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="I10" s="6" t="s">
-        <v>6</v>
+      <c r="I10" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
-        <v>33</v>
+      <c r="K10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -737,117 +758,131 @@
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>45336</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="8" t="s">
-        <v>40</v>
+      <c r="I12" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
-      <c r="I13" s="8" t="s">
-        <v>42</v>
+      <c r="I13" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G14" s="1"/>
       <c r="I14" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
-      <c r="I15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="I15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45331</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G16" s="1"/>
       <c r="I16" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
-      <c r="I17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="5">
-        <v>45331</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="I17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G18" s="1"/>
-      <c r="I18" s="6" t="s">
-        <v>11</v>
+      <c r="I18" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G19" s="1"/>
-      <c r="I19" s="6" t="s">
-        <v>12</v>
+      <c r="I19" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G20" s="1"/>
       <c r="I20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G21" s="1"/>
       <c r="I21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" s="5">
         <v>45334</v>
@@ -858,41 +893,49 @@
     <row r="22" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G22" s="1"/>
       <c r="I22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="K22" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G23" s="1"/>
       <c r="I23" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
       <c r="I24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
       <c r="I25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="L25" s="4"/>
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.3">
       <c r="I26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J26" s="5">
         <v>45335</v>
@@ -902,18 +945,22 @@
     </row>
     <row r="27" spans="7:12" x14ac:dyDescent="0.3">
       <c r="I27" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J27" s="5"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L27" s="4"/>
     </row>
     <row r="28" spans="7:12" x14ac:dyDescent="0.3">
       <c r="I28" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L28" s="4"/>
     </row>
   </sheetData>

</xml_diff>